<commit_message>
Added the rfid tag values to the voters table
</commit_message>
<xml_diff>
--- a/utils/frontend_test.xlsx
+++ b/utils/frontend_test.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dokumente\Projektmanagement\yourChoiceHO\Documentation\Feindesign\csv-mockup\frontend\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\projects\your-choice\utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12375" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12375"/>
   </bookViews>
   <sheets>
     <sheet name="voter" sheetId="1" r:id="rId1"/>
@@ -792,10 +792,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1161,6 +1161,31 @@
       </c>
       <c r="E21">
         <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C22">
+        <v>3754085</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C23">
+        <v>3756206</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C24">
+        <v>3765388</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C25">
+        <v>3813034</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C26">
+        <v>3873915</v>
       </c>
     </row>
   </sheetData>
@@ -2087,7 +2112,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>

</xml_diff>